<commit_message>
Remove password trigger jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>URL</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>apple x</t>
-  </si>
-  <si>
-    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -446,9 +443,7 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add password trigger jenkins
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>URL</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>apple x</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,9 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
add jennikns# Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="16725" windowHeight="7095"/>
@@ -11,7 +11,7 @@
     <sheet name="campaign" sheetId="2" r:id="rId2"/>
     <sheet name="lead" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -30,9 +30,6 @@
     <t>rashmi@dell.com</t>
   </si>
   <si>
-    <t>http://172.16.213.129:8080/crm/ShowHomePage.do</t>
-  </si>
-  <si>
     <t>Company Name</t>
   </si>
   <si>
@@ -64,13 +61,16 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>http://192.168.235.128:8080/crm/ShowHomePage.do</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,7 +202,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,7 +236,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -413,28 +411,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -442,12 +440,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -459,65 +457,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>